<commit_message>
refactor del calculo de riesgo y pureza proporcion
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/con_isolation/log_pcsmote_x_muestra_glass_D25_R25_PPproporcion.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/con_isolation/log_pcsmote_x_muestra_glass_D25_R25_PPproporcion.xlsx
@@ -657,7 +657,7 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -747,7 +747,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -833,7 +833,7 @@
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -919,7 +919,7 @@
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1525,7 +1525,7 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1783,7 +1783,7 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1869,7 +1869,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -1955,7 +1955,7 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2041,7 +2041,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2475,7 +2475,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2561,7 +2561,7 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2733,7 +2733,7 @@
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2819,7 +2819,7 @@
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2905,7 +2905,7 @@
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -2991,7 +2991,7 @@
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3163,7 +3163,7 @@
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3335,7 +3335,7 @@
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3507,7 +3507,7 @@
       <c r="Y35" t="inlineStr"/>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3593,7 +3593,7 @@
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3679,7 +3679,7 @@
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3851,7 +3851,7 @@
       <c r="Y39" t="inlineStr"/>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -3937,7 +3937,7 @@
       <c r="Y40" t="inlineStr"/>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4023,7 +4023,7 @@
       <c r="Y41" t="inlineStr"/>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.119569</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
       <c r="Y42" t="inlineStr"/>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4195,7 +4195,7 @@
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
       <c r="Y44" t="inlineStr"/>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4367,7 +4367,7 @@
       <c r="Y45" t="inlineStr"/>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4453,7 +4453,7 @@
       <c r="Y46" t="inlineStr"/>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4539,7 +4539,7 @@
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4625,7 +4625,7 @@
       <c r="Y48" t="inlineStr"/>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       <c r="Y49" t="inlineStr"/>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4801,7 +4801,7 @@
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4887,7 +4887,7 @@
       <c r="Y51" t="inlineStr"/>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -4973,7 +4973,7 @@
       <c r="Y52" t="inlineStr"/>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.135450</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -5059,7 +5059,7 @@
       <c r="Y53" t="inlineStr"/>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.136463</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.136463</t>
+          <t>2025-11-05T14:13:28.231820</t>
         </is>
       </c>
     </row>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.330054</t>
         </is>
       </c>
     </row>
@@ -5325,7 +5325,7 @@
       <c r="Y56" t="inlineStr"/>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.331115</t>
         </is>
       </c>
     </row>
@@ -5415,7 +5415,7 @@
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.331115</t>
         </is>
       </c>
     </row>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="Z58" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -5595,7 +5595,7 @@
       </c>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -5685,7 +5685,7 @@
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="Z61" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="Z62" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.151229</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -5951,7 +5951,7 @@
       <c r="Y63" t="inlineStr"/>
       <c r="Z63" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.152222</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -6037,7 +6037,7 @@
       <c r="Y64" t="inlineStr"/>
       <c r="Z64" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.152222</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -6123,7 +6123,7 @@
       <c r="Y65" t="inlineStr"/>
       <c r="Z65" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.152222</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -6213,7 +6213,7 @@
       </c>
       <c r="Z66" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.152222</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>
@@ -6299,7 +6299,7 @@
       <c r="Y67" t="inlineStr"/>
       <c r="Z67" t="inlineStr">
         <is>
-          <t>2025-11-05T11:16:27.152222</t>
+          <t>2025-11-05T14:13:28.331625</t>
         </is>
       </c>
     </row>

</xml_diff>